<commit_message>
Fairness with example ipynb
</commit_message>
<xml_diff>
--- a/src/sbe_vallib/table/pipelines/fairness_config.xlsx
+++ b/src/sbe_vallib/table/pipelines/fairness_config.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>import_path</t>
   </si>
@@ -68,7 +68,13 @@
     <t xml:space="preserve">Например, уровень дохода может быть связан с местом жительства клиента. Большой Джини в данном случае является показателем того, что по остальным факторам можно хорошо разделять данную переменную. Соответственно, исключение данного фактора не приведет к потере информации относительно связи целевой переменной и остальных факторов, не являющихся дискриминирующими. Так, существуют обоснованные отличия внутри защищенной характеристики, не связанные с ней напрямую. </t>
   </si>
   <si>
-    <t>Информативный тест</t>
+    <t>Не проверяет на дискриминацию</t>
+  </si>
+  <si>
+    <t>Не выставляется</t>
+  </si>
+  <si>
+    <t>Иначе</t>
   </si>
   <si>
     <t>sbe_vallib.table.fairness.test_target_rate_delta.test_target_rate_delta</t>
@@ -157,6 +163,24 @@
     <t>В остальных случаях</t>
   </si>
   <si>
+    <t>sbe_vallib.table.fairness.test_delete_protected.test_delete_protected</t>
+  </si>
+  <si>
+    <t>test_delete_protected</t>
+  </si>
+  <si>
+    <t>{'main_metric': 'gini', 'copy_model': True, 'df_index': 0, 'bad_semaphores': ['yellow', 'red'], 'feature_col': 'Защищенная характеристика', 'semaphore_col': 'Результат теста'}</t>
+  </si>
+  <si>
+    <t>Тест 7.5 Сравнение качества модели с дискриминирующими признаками и без них</t>
+  </si>
+  <si>
+    <t>бла</t>
+  </si>
+  <si>
+    <t>Тест информативный</t>
+  </si>
+  <si>
     <t>print_name</t>
   </si>
   <si>
@@ -225,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -236,14 +260,23 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -546,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -560,14 +593,14 @@
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
+      <c r="K2" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -587,35 +620,35 @@
     </row>
     <row r="3" ht="141.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>0.0</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -635,35 +668,35 @@
     </row>
     <row r="4" ht="78.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>28</v>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>0.0</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="7" t="s">
         <v>34</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -683,35 +716,35 @@
     </row>
     <row r="5" ht="378.0" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <v>0.0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>42</v>
+      <c r="K5" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -730,17 +763,37 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="I6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -7555,17 +7608,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>43</v>
+      <c r="B1" s="10" t="s">
+        <v>51</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>44</v>
+      <c r="C1" s="10" t="s">
+        <v>52</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -7586,17 +7639,17 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>45</v>
+      <c r="B2" s="10" t="s">
+        <v>53</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>46</v>
+      <c r="C2" s="10" t="s">
+        <v>54</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -7617,11 +7670,11 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -7642,11 +7695,11 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -7667,11 +7720,11 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -7692,11 +7745,11 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -7717,11 +7770,11 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -7742,11 +7795,11 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -7767,11 +7820,11 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -7792,11 +7845,11 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>

</xml_diff>